<commit_message>
proper folder structure added
</commit_message>
<xml_diff>
--- a/E-tollAcquiringSettlement/Processing/2025/09/25/ERROR_ETOLL_ACQUIRING_VOUCHER_250925_N1.xlsx
+++ b/E-tollAcquiringSettlement/Processing/2025/09/25/ERROR_ETOLL_ACQUIRING_VOUCHER_250925_N1.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="41">
   <si>
     <t>Account No</t>
   </si>
@@ -321,7 +321,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="n" s="0">
-        <v>495.0</v>
+        <v>0.0</v>
       </c>
       <c r="D10" t="s" s="0">
         <v>14</v>
@@ -474,7 +474,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -564,10 +564,10 @@
         <v>39</v>
       </c>
       <c r="C6" t="n" s="0">
-        <v>495.0</v>
+        <v>11120.0</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>14</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7">
@@ -578,10 +578,10 @@
         <v>39</v>
       </c>
       <c r="C7" t="n" s="0">
-        <v>11120.0</v>
+        <v>197810.77</v>
       </c>
       <c r="D7" t="s" s="0">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8">
@@ -592,35 +592,35 @@
         <v>39</v>
       </c>
       <c r="C8" t="n" s="0">
-        <v>197810.77</v>
+        <v>54324.0</v>
       </c>
       <c r="D8" t="s" s="0">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s" s="0">
         <v>39</v>
       </c>
       <c r="C9" t="n" s="0">
-        <v>54324.0</v>
+        <v>24.44</v>
       </c>
       <c r="D9" t="s" s="0">
-        <v>29</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s" s="0">
         <v>39</v>
       </c>
       <c r="C10" t="n" s="0">
-        <v>24.44</v>
+        <v>4.4</v>
       </c>
       <c r="D10" t="s" s="0">
         <v>10</v>
@@ -628,13 +628,13 @@
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C11" t="n" s="0">
-        <v>4.4</v>
+        <v>207277.77</v>
       </c>
       <c r="D11" t="s" s="0">
         <v>10</v>
@@ -642,29 +642,15 @@
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s" s="0">
         <v>40</v>
       </c>
       <c r="C12" t="n" s="0">
-        <v>207277.77</v>
+        <v>37310.0</v>
       </c>
       <c r="D12" t="s" s="0">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s" s="0">
-        <v>33</v>
-      </c>
-      <c r="B13" t="s" s="0">
-        <v>40</v>
-      </c>
-      <c r="C13" t="n" s="0">
-        <v>37310.0</v>
-      </c>
-      <c r="D13" t="s" s="0">
         <v>10</v>
       </c>
     </row>

</xml_diff>